<commit_message>
added checkstyle total erros for SO.ru, changed ktlint boxplot
</commit_message>
<xml_diff>
--- a/StatisticalAnalysis/Ktlint/ktlint_question_answers_errors.xlsx
+++ b/StatisticalAnalysis/Ktlint/ktlint_question_answers_errors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibamberg-my.sharepoint.com/personal/fabian_ulrich_stud_uni-bamberg_de/Documents/SS 20/Bachelorarbeit/Code Quality analysis/Bachelor-Thesis/StatisticalAnalysis/Ktlint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{332AA524-B70A-45F8-87C7-370BD91416BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{332AA524-B70A-45F8-87C7-370BD91416BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E5DE32AA-5418-4B07-8336-4B3AEE9913C6}"/>
   <bookViews>
-    <workbookView xWindow="5655" yWindow="2325" windowWidth="21600" windowHeight="11325" xr2:uid="{9829E879-C1B9-40C0-BF18-E5A29EE8BA51}"/>
+    <workbookView xWindow="4290" yWindow="5685" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{9829E879-C1B9-40C0-BF18-E5A29EE8BA51}"/>
   </bookViews>
   <sheets>
     <sheet name="ktlint_question_error_score" sheetId="4" r:id="rId1"/>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D69DFB-90CC-4DCA-B8BD-D92AE6B3B455}">
   <dimension ref="A1:G322"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4130,8 +4130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC00DC3-6291-474D-BE85-39E96695EEA5}">
   <dimension ref="A1:G170"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4212,8 +4212,8 @@
         <v>7</v>
       </c>
       <c r="E4">
-        <f>SUM(C2:C47)</f>
-        <v>237</v>
+        <f>SUM(C2:C46)</f>
+        <v>236</v>
       </c>
       <c r="F4">
         <f>SUM(C47:C149)</f>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="E5">
         <f>E4/E3</f>
-        <v>5.2666666666666666</v>
+        <v>5.2444444444444445</v>
       </c>
       <c r="F5">
         <f>F4/F3</f>
@@ -4264,8 +4264,8 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <f>MEDIAN(C2:C47)</f>
-        <v>3</v>
+        <f>MEDIAN(C2:C46)</f>
+        <v>4</v>
       </c>
       <c r="F6">
         <f>MEDIAN(C47:C149)</f>

</xml_diff>